<commit_message>
Finished for the presentation
</commit_message>
<xml_diff>
--- a/Visualizer/Clean lines/valores vacio Nave NIR_prueba3.xlsx
+++ b/Visualizer/Clean lines/valores vacio Nave NIR_prueba3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clauw\Documents\Programming\Final-Project\Visualizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clauw\Documents\Programming\Final-Project\Visualizer\Clean lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DD3BE9-60BA-432D-B2FC-9156BC9E5F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C0AC96-0C95-4A6F-BDA8-7D3FAB8A5632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="1692" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,7 +387,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>